<commit_message>
Fixed fb_usb2_ba connector A USB connector holes.
</commit_message>
<xml_diff>
--- a/eagle/fp_usb2_ba/fp_usb2_ba_bom.xlsx
+++ b/eagle/fp_usb2_ba/fp_usb2_ba_bom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="All" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bottom" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="All" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Top" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Bottom" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -600,7 +600,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2022 September 15</t>
+          <t>2022 September 28</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>JS220_fp_usb2_ba_pcb_revA</t>
+          <t>JS220_fp_usb2_ba_pcb_revB</t>
         </is>
       </c>
     </row>
@@ -743,7 +743,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2022 September 15</t>
+          <t>2022 September 28</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>JS220_fp_usb2_ba_pcb_revA</t>
+          <t>JS220_fp_usb2_ba_pcb_revB</t>
         </is>
       </c>
     </row>
@@ -886,7 +886,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2022 September 15</t>
+          <t>2022 September 28</t>
         </is>
       </c>
     </row>

</xml_diff>